<commit_message>
changed exercise 13 to 9
</commit_message>
<xml_diff>
--- a/data/survey_data/combined_data/sat_data_combined.xlsx
+++ b/data/survey_data/combined_data/sat_data_combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weijiechua/Desktop/ImperialClasses/Courses/thirdterm/individual/official/official_sat_chatbot/data/survey_data/combined_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17E1963-2B08-2845-9D92-C42E3FAD5D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB381661-2AB6-E040-8364-C64E465DB142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,9 +223,6 @@
     <t>Is the emotion positive or negative?</t>
   </si>
   <si>
-    <t>Let us practice Exercise 13 to overcome negative emotions.</t>
-  </si>
-  <si>
     <t>Do you feel compassionate toward your childhood self?</t>
   </si>
   <si>
@@ -400,9 +397,6 @@
     <t>Do you feel more positive or negative?</t>
   </si>
   <si>
-    <t>Let us start practicing Exercise 13 to overcome negative emotions.</t>
-  </si>
-  <si>
     <t>Do you feel you are compassionate towards your childhood self?</t>
   </si>
   <si>
@@ -556,9 +550,6 @@
     <t>Do you think that you are feeling more positively or negatively?</t>
   </si>
   <si>
-    <t>Now, let's take a moment to go through Exercise 13 so that I can help you better understand how to overcome any negative feelings that you might be experiencing.</t>
-  </si>
-  <si>
     <t>That's wonderful to hear. Between protecting your childhood self and wanting your childhood self to grow stronger from adversities, which one do you think more accurately describes your feelings?</t>
   </si>
   <si>
@@ -706,9 +697,6 @@
     <t>Do you feel good or bad?</t>
   </si>
   <si>
-    <t>Let's try Exercise 13 to see if it helps!</t>
-  </si>
-  <si>
     <t>Do you feel compassion towards your childhood self?</t>
   </si>
   <si>
@@ -874,9 +862,6 @@
     <t>Are you feeling positive or negative?</t>
   </si>
   <si>
-    <t>Let’s do Exercise 13 together to get over the negative emotions you’re feeling.</t>
-  </si>
-  <si>
     <t>Cool! Do you feel like protecting your childhood self or do you think he/she should toughen up?</t>
   </si>
   <si>
@@ -1009,9 +994,6 @@
     <t>Is the emotion a positive one or a negative one?</t>
   </si>
   <si>
-    <t>Let’s go through Exercise 13 so we can solve this together!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Do you feel like you have compassion for your childhood self? </t>
   </si>
   <si>
@@ -1160,9 +1142,6 @@
   </si>
   <si>
     <t>Would you say the emotion is positive or negative?</t>
-  </si>
-  <si>
-    <t>Let's practice Exercise 13 to learn ways of overcoming negative emotions.</t>
   </si>
   <si>
     <t>Congratulations! You have shown tender compassion. Tender compassion is the first phase of compassion, where you feel sympathy towards the victim. You feel for the victim, hoping to do something that can help alleviate their suffering.</t>
@@ -1637,9 +1616,6 @@
     <t>May I know how you're feeling today?</t>
   </si>
   <si>
-    <t>I think you should try Exercise 13, it will be very helpful for you in overcoming your negative emotions!</t>
-  </si>
-  <si>
     <t xml:space="preserve">How do you feel towards your childhood self? Do you feel compassionate? </t>
   </si>
   <si>
@@ -1682,9 +1658,6 @@
     <t>Do you feel that in a positive or negative way?</t>
   </si>
   <si>
-    <t>We will practice Exercise 13 together now to help with your negative feelings.</t>
-  </si>
-  <si>
     <t>How do you feel about your childhood self? Do you feel compassionate?</t>
   </si>
   <si>
@@ -1733,9 +1706,6 @@
     <t>Can you tell if the emotion is positive or negative?</t>
   </si>
   <si>
-    <t>For overcoming negative emotions, let us practice the Exercise 13 below.</t>
-  </si>
-  <si>
     <t>Can you relate to your childhood self in a compassionate way?</t>
   </si>
   <si>
@@ -1806,15 +1776,6 @@
   </si>
   <si>
     <t>Are your emotions positive or negative?</t>
-  </si>
-  <si>
-    <t>Let us go through Exercise 13 to help you cope with how you feel.</t>
-  </si>
-  <si>
-    <t>Please complete Exercise 13 and we can get past any negative emotions together.</t>
-  </si>
-  <si>
-    <t>Would you like to practice Exercise 13? This exercise may help you overcome your negative emotions.</t>
   </si>
   <si>
     <t>How do you feel about your childhood?</t>
@@ -2180,6 +2141,45 @@
   </si>
   <si>
     <t>Many thanks for your cooperation. I hope to see you again soon.</t>
+  </si>
+  <si>
+    <t>Let us start practicing Exercise 9 to overcome negative emotions.</t>
+  </si>
+  <si>
+    <t>Now, let's take a moment to go through Exercise 9 so that I can help you better understand how to overcome any negative feelings that you might be experiencing.</t>
+  </si>
+  <si>
+    <t>Let's try Exercise 9 to see if it helps!</t>
+  </si>
+  <si>
+    <t>Let’s do Exercise 9 together to get over the negative emotions you’re feeling.</t>
+  </si>
+  <si>
+    <t>Let’s go through Exercise 9 so we can solve this together!</t>
+  </si>
+  <si>
+    <t>Let's practice Exercise 9 to learn ways of overcoming negative emotions.</t>
+  </si>
+  <si>
+    <t>Let us go through Exercise 9 to help you cope with how you feel.</t>
+  </si>
+  <si>
+    <t>Please complete Exercise 9 and we can get past any negative emotions together.</t>
+  </si>
+  <si>
+    <t>Would you like to practice Exercise 9? This exercise may help you overcome your negative emotions.</t>
+  </si>
+  <si>
+    <t>I think you should try Exercise 9, it will be very helpful for you in overcoming your negative emotions!</t>
+  </si>
+  <si>
+    <t>We will practice Exercise 9 together now to help with your negative feelings.</t>
+  </si>
+  <si>
+    <t>For overcoming negative emotions, let us practice the Exercise 9 below.</t>
+  </si>
+  <si>
+    <t>Let us practice Exercise 9 to overcome negative emotions.</t>
   </si>
 </sst>
 </file>
@@ -2565,8 +2565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BL13" zoomScale="125" workbookViewId="0">
-      <selection activeCell="BN2" sqref="BN2:BN25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2823,7 +2823,7 @@
         <v>63</v>
       </c>
       <c r="BN1" s="4" t="s">
-        <v>694</v>
+        <v>681</v>
       </c>
     </row>
     <row r="2" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -2840,190 +2840,190 @@
         <v>66</v>
       </c>
       <c r="E2" t="s">
+        <v>718</v>
+      </c>
+      <c r="F2" t="s">
         <v>67</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>68</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" t="s">
         <v>75</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>76</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" t="s">
         <v>78</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" t="s">
         <v>80</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" t="s">
         <v>86</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" t="s">
         <v>88</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" t="s">
         <v>92</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" t="s">
         <v>94</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>95</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AM2" t="s">
+        <v>643</v>
+      </c>
+      <c r="AN2" t="s">
         <v>100</v>
       </c>
-      <c r="AM2" t="s">
-        <v>656</v>
-      </c>
-      <c r="AN2" t="s">
+      <c r="AO2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AQ2" t="s">
         <v>103</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>104</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>105</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AU2" t="s">
+        <v>647</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>648</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>679</v>
+      </c>
+      <c r="AX2" t="s">
         <v>107</v>
       </c>
-      <c r="AU2" t="s">
-        <v>660</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>661</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>692</v>
-      </c>
-      <c r="AX2" t="s">
+      <c r="AY2" t="s">
         <v>108</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="BA2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="BA2" s="3" t="s">
+      <c r="BB2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="BB2" s="3" t="s">
+      <c r="BC2" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="BC2" s="3" t="s">
+      <c r="BD2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="BD2" s="3" t="s">
+      <c r="BE2" t="s">
         <v>114</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BF2" t="s">
         <v>115</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BG2" t="s">
         <v>116</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BH2" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="BH2" s="3" t="s">
+      <c r="BI2" t="s">
+        <v>367</v>
+      </c>
+      <c r="BJ2" t="s">
         <v>118</v>
       </c>
-      <c r="BI2" t="s">
-        <v>373</v>
-      </c>
-      <c r="BJ2" t="s">
+      <c r="BK2" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="BK2" s="3" t="s">
+      <c r="BL2" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="BL2" s="3" t="s">
+      <c r="BM2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="BM2" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="BN2" t="s">
-        <v>695</v>
+        <v>682</v>
       </c>
     </row>
     <row r="3" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -3031,199 +3031,199 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
         <v>123</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>124</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>706</v>
+      </c>
+      <c r="F3" t="s">
         <v>125</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>126</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>607</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>610</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="N3" t="s">
         <v>130</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="O3" t="s">
         <v>131</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="P3" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>132</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="S3" t="s">
         <v>617</v>
       </c>
-      <c r="N3" t="s">
-        <v>132</v>
-      </c>
-      <c r="O3" t="s">
-        <v>133</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="T3" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="U3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="S3" t="s">
+      <c r="X3" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y3" t="s">
         <v>630</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="W3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>634</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="AC3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="Y3" t="s">
-        <v>643</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>645</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>647</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AE3" t="s">
         <v>139</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AG3" t="s">
         <v>141</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AH3" t="s">
         <v>142</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AI3" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="AI3" s="3" t="s">
+      <c r="AK3" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="AJ3" s="3" t="s">
+      <c r="AL3" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="AK3" s="3" t="s">
+      <c r="AM3" t="s">
         <v>147</v>
       </c>
-      <c r="AL3" s="3" t="s">
+      <c r="AN3" t="s">
         <v>148</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AO3" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AP3" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="AO3" s="3" t="s">
+      <c r="AQ3" t="s">
         <v>151</v>
       </c>
-      <c r="AP3" s="3" t="s">
+      <c r="AR3" t="s">
         <v>152</v>
       </c>
-      <c r="AQ3" t="s">
+      <c r="AS3" t="s">
         <v>153</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="AT3" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AU3" t="s">
         <v>155</v>
       </c>
-      <c r="AT3" s="3" t="s">
+      <c r="AV3" t="s">
         <v>156</v>
       </c>
-      <c r="AU3" t="s">
+      <c r="AW3" t="s">
+        <v>680</v>
+      </c>
+      <c r="AX3" t="s">
         <v>157</v>
       </c>
-      <c r="AV3" t="s">
+      <c r="AY3" t="s">
         <v>158</v>
       </c>
-      <c r="AW3" t="s">
-        <v>693</v>
-      </c>
-      <c r="AX3" t="s">
+      <c r="AZ3" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="AY3" t="s">
+      <c r="BA3" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="AZ3" s="3" t="s">
+      <c r="BB3" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="BA3" s="3" t="s">
+      <c r="BC3" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="BB3" s="3" t="s">
+      <c r="BD3" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="BC3" s="3" t="s">
+      <c r="BE3" t="s">
         <v>164</v>
       </c>
-      <c r="BD3" s="3" t="s">
+      <c r="BF3" t="s">
         <v>165</v>
       </c>
-      <c r="BE3" t="s">
+      <c r="BG3" t="s">
         <v>166</v>
       </c>
-      <c r="BF3" t="s">
+      <c r="BH3" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="BG3" t="s">
+      <c r="BI3" t="s">
         <v>168</v>
       </c>
-      <c r="BH3" s="3" t="s">
+      <c r="BJ3" t="s">
         <v>169</v>
       </c>
-      <c r="BI3" t="s">
+      <c r="BK3" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="BJ3" t="s">
+      <c r="BL3" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="BK3" s="3" t="s">
+      <c r="BM3" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="BL3" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="BM3" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="BN3" t="s">
-        <v>696</v>
+        <v>683</v>
       </c>
     </row>
     <row r="4" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -3231,199 +3231,199 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" t="s">
         <v>175</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
+        <v>707</v>
+      </c>
+      <c r="F4" t="s">
+        <v>665</v>
+      </c>
+      <c r="G4" t="s">
         <v>176</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E4" t="s">
+      <c r="I4" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F4" t="s">
-        <v>678</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="J4" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="N4" t="s">
         <v>183</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="O4" t="s">
         <v>184</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="P4" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="Q4" t="s">
         <v>185</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="O4" t="s">
+      <c r="S4" t="s">
+        <v>615</v>
+      </c>
+      <c r="T4" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="U4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="V4" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="S4" t="s">
-        <v>628</v>
-      </c>
-      <c r="T4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="U4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="V4" s="3" t="s">
+      <c r="Y4" t="s">
         <v>191</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="AA4" t="s">
         <v>193</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AB4" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AD4" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AE4" t="s">
         <v>197</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AG4" t="s">
         <v>199</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AH4" t="s">
         <v>200</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AK4" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AM4" t="s">
         <v>205</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AN4" t="s">
         <v>206</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AP4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ4" t="s">
         <v>208</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AR4" t="s">
         <v>209</v>
       </c>
-      <c r="AO4" s="3" t="s">
+      <c r="AS4" t="s">
         <v>210</v>
       </c>
-      <c r="AP4" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AQ4" t="s">
+      <c r="AT4" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="AU4" t="s">
         <v>211</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AV4" t="s">
         <v>212</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AW4" t="s">
+        <v>679</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AY4" t="s">
         <v>213</v>
       </c>
-      <c r="AT4" s="3" t="s">
-        <v>659</v>
-      </c>
-      <c r="AU4" t="s">
+      <c r="AZ4" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="BA4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="BB4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="BC4" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="BD4" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="AW4" t="s">
-        <v>692</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>108</v>
-      </c>
-      <c r="AY4" t="s">
+      <c r="BE4" t="s">
         <v>216</v>
       </c>
-      <c r="AZ4" s="3" t="s">
-        <v>665</v>
-      </c>
-      <c r="BA4" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="BB4" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="BC4" s="3" t="s">
+      <c r="BF4" t="s">
         <v>217</v>
       </c>
-      <c r="BD4" s="3" t="s">
+      <c r="BG4" t="s">
+        <v>116</v>
+      </c>
+      <c r="BH4" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="BE4" t="s">
+      <c r="BI4" t="s">
+        <v>525</v>
+      </c>
+      <c r="BJ4" t="s">
         <v>219</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BK4" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="BG4" t="s">
-        <v>117</v>
-      </c>
-      <c r="BH4" s="3" t="s">
+      <c r="BL4" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="BM4" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="BI4" t="s">
-        <v>532</v>
-      </c>
-      <c r="BJ4" t="s">
-        <v>222</v>
-      </c>
-      <c r="BK4" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="BL4" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="BM4" s="3" t="s">
-        <v>224</v>
-      </c>
       <c r="BN4" t="s">
-        <v>697</v>
+        <v>684</v>
       </c>
     </row>
     <row r="5" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -3431,199 +3431,199 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E5" t="s">
+        <v>708</v>
+      </c>
+      <c r="F5" t="s">
         <v>225</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>226</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H5" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F5" t="s">
+      <c r="K5" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="G5" t="s">
+      <c r="L5" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>585</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="N5" t="s">
         <v>232</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="O5" t="s">
         <v>233</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="Q5" t="s">
         <v>235</v>
       </c>
-      <c r="N5" t="s">
+      <c r="R5" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="O5" t="s">
+      <c r="S5" t="s">
+        <v>616</v>
+      </c>
+      <c r="T5" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="U5" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="V5" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="W5" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="X5" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="S5" t="s">
-        <v>629</v>
-      </c>
-      <c r="T5" s="3" t="s">
+      <c r="Y5" t="s">
         <v>241</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="Z5" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="AA5" t="s">
         <v>242</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="AB5" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="X5" s="3" t="s">
+      <c r="AC5" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="AD5" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="Z5" s="3" t="s">
+      <c r="AE5" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="AK5" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="AL5" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO5" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AP5" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>257</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>258</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AT5" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="AA5" t="s">
-        <v>246</v>
-      </c>
-      <c r="AB5" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="AC5" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>250</v>
-      </c>
-      <c r="AF5" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>253</v>
-      </c>
-      <c r="AI5" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="AJ5" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="AK5" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="AL5" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>258</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>101</v>
-      </c>
-      <c r="AO5" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="AP5" s="3" t="s">
+      <c r="AU5" t="s">
         <v>260</v>
       </c>
-      <c r="AQ5" t="s">
-        <v>261</v>
-      </c>
-      <c r="AR5" t="s">
+      <c r="AV5" t="s">
+        <v>649</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>674</v>
+      </c>
+      <c r="AX5" t="s">
         <v>262</v>
       </c>
-      <c r="AS5" t="s">
-        <v>106</v>
-      </c>
-      <c r="AT5" s="3" t="s">
-        <v>659</v>
-      </c>
-      <c r="AU5" t="s">
+      <c r="AY5" t="s">
+        <v>263</v>
+      </c>
+      <c r="AZ5" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="AV5" t="s">
-        <v>662</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>687</v>
-      </c>
-      <c r="AX5" t="s">
+      <c r="BA5" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="BB5" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="AY5" t="s">
+      <c r="BC5" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="AZ5" s="3" t="s">
+      <c r="BD5" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="BA5" s="3" t="s">
-        <v>666</v>
-      </c>
-      <c r="BB5" s="3" t="s">
+      <c r="BE5" t="s">
+        <v>657</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>269</v>
+      </c>
+      <c r="BG5" t="s">
         <v>270</v>
       </c>
-      <c r="BC5" s="3" t="s">
+      <c r="BH5" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="BD5" s="3" t="s">
+      <c r="BI5" t="s">
         <v>272</v>
       </c>
-      <c r="BE5" t="s">
-        <v>670</v>
-      </c>
-      <c r="BF5" t="s">
+      <c r="BJ5" t="s">
         <v>273</v>
       </c>
-      <c r="BG5" t="s">
+      <c r="BK5" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="BH5" s="3" t="s">
+      <c r="BL5" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="BI5" t="s">
+      <c r="BM5" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="BJ5" t="s">
-        <v>277</v>
-      </c>
-      <c r="BK5" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="BL5" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="BM5" s="3" t="s">
-        <v>280</v>
-      </c>
       <c r="BN5" t="s">
-        <v>698</v>
+        <v>685</v>
       </c>
     </row>
     <row r="6" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -3631,199 +3631,199 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D6" t="s">
+        <v>279</v>
+      </c>
+      <c r="E6" t="s">
+        <v>709</v>
+      </c>
+      <c r="F6" t="s">
+        <v>585</v>
+      </c>
+      <c r="G6" t="s">
+        <v>280</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="C6" t="s">
+      <c r="I6" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D6" t="s">
+      <c r="L6" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="E6" t="s">
+      <c r="M6" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="N6" t="s">
         <v>284</v>
       </c>
-      <c r="F6" t="s">
-        <v>598</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="O6" t="s">
+        <v>184</v>
+      </c>
+      <c r="P6" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="Q6" t="s">
         <v>286</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="R6" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="S6" t="s">
         <v>287</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>618</v>
-      </c>
-      <c r="N6" t="s">
-        <v>289</v>
-      </c>
-      <c r="O6" t="s">
-        <v>187</v>
-      </c>
-      <c r="P6" s="3" t="s">
+      <c r="U6" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="W6" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="X6" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="R6" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="S6" t="s">
-        <v>292</v>
-      </c>
-      <c r="T6" s="3" t="s">
+      <c r="Y6" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>635</v>
+      </c>
+      <c r="AB6" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="U6" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="W6" s="3" t="s">
+      <c r="AC6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="AE6" t="s">
         <v>295</v>
       </c>
-      <c r="X6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="Y6" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z6" s="3" t="s">
+      <c r="AG6" t="s">
+        <v>297</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>298</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>644</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO6" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AP6" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>303</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>304</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>305</v>
+      </c>
+      <c r="AT6" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="AA6" t="s">
-        <v>648</v>
-      </c>
-      <c r="AB6" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="AC6" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>300</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>302</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>303</v>
-      </c>
-      <c r="AI6" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="AJ6" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="AK6" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AL6" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>657</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>101</v>
-      </c>
-      <c r="AO6" s="3" t="s">
+      <c r="AU6" t="s">
         <v>306</v>
       </c>
-      <c r="AP6" s="3" t="s">
+      <c r="AV6" t="s">
+        <v>650</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>673</v>
+      </c>
+      <c r="AX6" t="s">
         <v>307</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="AY6" t="s">
         <v>308</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AZ6" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="BA6" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="AT6" s="3" t="s">
-        <v>659</v>
-      </c>
-      <c r="AU6" t="s">
+      <c r="BB6" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="AV6" t="s">
-        <v>663</v>
-      </c>
-      <c r="AW6" t="s">
+      <c r="BC6" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="BD6" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="BE6" t="s">
+        <v>658</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>313</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>314</v>
+      </c>
+      <c r="BH6" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>662</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>317</v>
+      </c>
+      <c r="BK6" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="BL6" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="BM6" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="BN6" t="s">
         <v>686</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>312</v>
-      </c>
-      <c r="AY6" t="s">
-        <v>313</v>
-      </c>
-      <c r="AZ6" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="BA6" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="BB6" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="BC6" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="BD6" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="BE6" t="s">
-        <v>671</v>
-      </c>
-      <c r="BF6" t="s">
-        <v>318</v>
-      </c>
-      <c r="BG6" t="s">
-        <v>319</v>
-      </c>
-      <c r="BH6" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="BI6" t="s">
-        <v>675</v>
-      </c>
-      <c r="BJ6" t="s">
-        <v>322</v>
-      </c>
-      <c r="BK6" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="BL6" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="BM6" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="BN6" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="7" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -3831,199 +3831,199 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C7" t="s">
+        <v>322</v>
+      </c>
+      <c r="D7" t="s">
+        <v>323</v>
+      </c>
+      <c r="E7" t="s">
+        <v>710</v>
+      </c>
+      <c r="F7" t="s">
+        <v>324</v>
+      </c>
+      <c r="G7" t="s">
+        <v>325</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="C7" t="s">
+      <c r="I7" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="D7" t="s">
+      <c r="J7" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="E7" t="s">
+      <c r="K7" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="F7" t="s">
+      <c r="L7" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G7" t="s">
+      <c r="M7" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="N7" t="s">
         <v>331</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="O7" t="s">
         <v>332</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="Q7" t="s">
         <v>334</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="R7" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="S7" t="s">
         <v>336</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>619</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="T7" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="O7" t="s">
+      <c r="U7" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="V7" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="W7" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="X7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z7" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="R7" s="3" t="s">
+      <c r="AA7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB7" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="S7" t="s">
+      <c r="AC7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF7" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="AG7" t="s">
         <v>343</v>
       </c>
-      <c r="U7" s="3" t="s">
+      <c r="AH7" t="s">
         <v>344</v>
       </c>
-      <c r="V7" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="W7" s="3" t="s">
+      <c r="AI7" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="X7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z7" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB7" s="3" t="s">
+      <c r="AJ7" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="AK7" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="AC7" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD7" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF7" s="3" t="s">
+      <c r="AL7" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="AM7" t="s">
         <v>348</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AN7" t="s">
         <v>349</v>
       </c>
-      <c r="AH7" t="s">
-        <v>350</v>
-      </c>
-      <c r="AI7" s="3" t="s">
+      <c r="AO7" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="AP7" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="AJ7" s="3" t="s">
-        <v>654</v>
-      </c>
-      <c r="AK7" s="3" t="s">
+      <c r="AQ7" t="s">
+        <v>352</v>
+      </c>
+      <c r="AR7" t="s">
         <v>353</v>
       </c>
-      <c r="AL7" s="3" t="s">
-        <v>681</v>
-      </c>
-      <c r="AM7" t="s">
+      <c r="AS7" t="s">
         <v>354</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AT7" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="AO7" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="AP7" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="AQ7" t="s">
+      <c r="AU7" t="s">
+        <v>356</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>651</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>672</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>576</v>
+      </c>
+      <c r="AY7" t="s">
         <v>358</v>
       </c>
-      <c r="AR7" t="s">
+      <c r="AZ7" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="AS7" t="s">
+      <c r="BA7" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="AT7" s="3" t="s">
+      <c r="BB7" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="AU7" t="s">
+      <c r="BC7" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="AV7" t="s">
-        <v>664</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>685</v>
-      </c>
-      <c r="AX7" t="s">
-        <v>586</v>
-      </c>
-      <c r="AY7" t="s">
+      <c r="BD7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="BE7" t="s">
+        <v>363</v>
+      </c>
+      <c r="BF7" t="s">
         <v>364</v>
       </c>
-      <c r="AZ7" s="3" t="s">
+      <c r="BG7" t="s">
         <v>365</v>
       </c>
-      <c r="BA7" s="3" t="s">
+      <c r="BH7" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="BB7" s="3" t="s">
+      <c r="BI7" t="s">
         <v>367</v>
       </c>
-      <c r="BC7" s="3" t="s">
+      <c r="BJ7" t="s">
         <v>368</v>
       </c>
-      <c r="BD7" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="BE7" t="s">
+      <c r="BK7" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="BF7" t="s">
+      <c r="BL7" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="BG7" t="s">
+      <c r="BM7" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="BH7" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="BI7" t="s">
-        <v>373</v>
-      </c>
-      <c r="BJ7" t="s">
-        <v>374</v>
-      </c>
-      <c r="BK7" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="BL7" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="BM7" s="3" t="s">
-        <v>377</v>
-      </c>
       <c r="BN7" t="s">
-        <v>700</v>
+        <v>687</v>
       </c>
     </row>
     <row r="8" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -4034,196 +4034,196 @@
         <v>64</v>
       </c>
       <c r="C8" t="s">
+        <v>372</v>
+      </c>
+      <c r="D8" t="s">
+        <v>373</v>
+      </c>
+      <c r="E8" t="s">
+        <v>711</v>
+      </c>
+      <c r="F8" t="s">
+        <v>666</v>
+      </c>
+      <c r="G8" t="s">
+        <v>587</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="N8" t="s">
+        <v>376</v>
+      </c>
+      <c r="O8" t="s">
+        <v>377</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="D8" t="s">
+      <c r="Q8" t="s">
+        <v>78</v>
+      </c>
+      <c r="R8" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="E8" t="s">
+      <c r="S8" t="s">
         <v>380</v>
       </c>
-      <c r="F8" t="s">
-        <v>679</v>
-      </c>
-      <c r="G8" t="s">
-        <v>600</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="T8" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="U8" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="W8" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>612</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>615</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>620</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="X8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>631</v>
+      </c>
+      <c r="Z8" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="O8" t="s">
+      <c r="AA8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="AC8" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="AD8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE8" t="s">
         <v>385</v>
       </c>
-      <c r="Q8" t="s">
-        <v>79</v>
-      </c>
-      <c r="R8" s="3" t="s">
+      <c r="AF8" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="S8" t="s">
+      <c r="AG8" t="s">
+        <v>667</v>
+      </c>
+      <c r="AH8" t="s">
         <v>387</v>
       </c>
-      <c r="T8" s="3" t="s">
+      <c r="AI8" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="AJ8" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="U8" s="3" t="s">
-        <v>635</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="W8" s="3" t="s">
+      <c r="AK8" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="X8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>644</v>
-      </c>
-      <c r="Z8" s="3" t="s">
+      <c r="AL8" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="AM8" t="s">
         <v>390</v>
       </c>
-      <c r="AA8" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB8" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="AC8" s="3" t="s">
+      <c r="AN8" t="s">
         <v>391</v>
       </c>
-      <c r="AD8" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AE8" t="s">
+      <c r="AO8" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="AF8" s="3" t="s">
+      <c r="AP8" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="AG8" t="s">
-        <v>680</v>
-      </c>
-      <c r="AH8" t="s">
+      <c r="AQ8" t="s">
         <v>394</v>
       </c>
-      <c r="AI8" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="AJ8" s="3" t="s">
+      <c r="AR8" t="s">
         <v>395</v>
       </c>
-      <c r="AK8" s="3" t="s">
+      <c r="AS8" t="s">
         <v>396</v>
       </c>
-      <c r="AL8" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="AM8" t="s">
+      <c r="AT8" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="AN8" t="s">
+      <c r="AU8" t="s">
         <v>398</v>
       </c>
-      <c r="AO8" s="3" t="s">
+      <c r="AV8" t="s">
         <v>399</v>
       </c>
-      <c r="AP8" s="3" t="s">
+      <c r="AW8" t="s">
+        <v>678</v>
+      </c>
+      <c r="AX8" t="s">
         <v>400</v>
       </c>
-      <c r="AQ8" t="s">
+      <c r="AY8" t="s">
         <v>401</v>
       </c>
-      <c r="AR8" t="s">
+      <c r="AZ8" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="AS8" t="s">
+      <c r="BA8" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="AT8" s="3" t="s">
+      <c r="BB8" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="AU8" t="s">
+      <c r="BC8" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="AV8" t="s">
+      <c r="BD8" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="AW8" t="s">
-        <v>691</v>
-      </c>
-      <c r="AX8" t="s">
+      <c r="BE8" t="s">
         <v>407</v>
       </c>
-      <c r="AY8" t="s">
+      <c r="BF8" t="s">
         <v>408</v>
       </c>
-      <c r="AZ8" s="3" t="s">
+      <c r="BG8" t="s">
         <v>409</v>
       </c>
-      <c r="BA8" s="3" t="s">
+      <c r="BH8" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="BI8" t="s">
         <v>410</v>
       </c>
-      <c r="BB8" s="3" t="s">
+      <c r="BJ8" t="s">
         <v>411</v>
       </c>
-      <c r="BC8" s="3" t="s">
+      <c r="BK8" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="BD8" s="3" t="s">
+      <c r="BL8" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="BE8" t="s">
+      <c r="BM8" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="BF8" t="s">
-        <v>415</v>
-      </c>
-      <c r="BG8" t="s">
-        <v>416</v>
-      </c>
-      <c r="BH8" s="3" t="s">
-        <v>674</v>
-      </c>
-      <c r="BI8" t="s">
-        <v>417</v>
-      </c>
-      <c r="BJ8" t="s">
-        <v>418</v>
-      </c>
-      <c r="BK8" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="BL8" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="BM8" s="3" t="s">
-        <v>421</v>
-      </c>
       <c r="BN8" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
     </row>
     <row r="9" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -4234,196 +4234,196 @@
         <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
       <c r="D9" t="s">
         <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>595</v>
+        <v>712</v>
       </c>
       <c r="F9" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
       <c r="G9" t="s">
+        <v>415</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="N9" t="s">
+        <v>75</v>
+      </c>
+      <c r="O9" t="s">
+        <v>419</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="S9" t="s">
         <v>422</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="T9" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="U9" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="V9" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="W9" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>621</v>
-      </c>
-      <c r="N9" t="s">
-        <v>76</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="X9" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="Y9" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z9" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="Q9" t="s">
-        <v>79</v>
-      </c>
-      <c r="R9" s="3" t="s">
+      <c r="AA9" t="s">
         <v>428</v>
       </c>
-      <c r="S9" t="s">
+      <c r="AB9" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="T9" s="3" t="s">
+      <c r="AC9" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="AD9" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="U9" s="3" t="s">
+      <c r="AE9" t="s">
         <v>431</v>
       </c>
-      <c r="V9" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="W9" s="3" t="s">
+      <c r="AF9" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="X9" s="3" t="s">
+      <c r="AG9" t="s">
         <v>433</v>
       </c>
-      <c r="Y9" t="s">
-        <v>245</v>
-      </c>
-      <c r="Z9" s="3" t="s">
+      <c r="AH9" t="s">
         <v>434</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AI9" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="AB9" s="3" t="s">
+      <c r="AJ9" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="AC9" s="3" t="s">
-        <v>651</v>
-      </c>
-      <c r="AD9" s="3" t="s">
+      <c r="AK9" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AL9" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="AF9" s="3" t="s">
+      <c r="AM9" t="s">
         <v>439</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AN9" t="s">
         <v>440</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AO9" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="AI9" s="3" t="s">
+      <c r="AP9" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="AJ9" s="3" t="s">
+      <c r="AQ9" t="s">
         <v>443</v>
       </c>
-      <c r="AK9" s="3" t="s">
+      <c r="AR9" t="s">
         <v>444</v>
       </c>
-      <c r="AL9" s="3" t="s">
+      <c r="AS9" t="s">
         <v>445</v>
       </c>
-      <c r="AM9" t="s">
+      <c r="AT9" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AU9" t="s">
         <v>447</v>
       </c>
-      <c r="AO9" s="3" t="s">
+      <c r="AV9" t="s">
         <v>448</v>
       </c>
-      <c r="AP9" s="3" t="s">
+      <c r="AW9" t="s">
+        <v>677</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>157</v>
+      </c>
+      <c r="AY9" t="s">
         <v>449</v>
       </c>
-      <c r="AQ9" t="s">
+      <c r="AZ9" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="AR9" t="s">
+      <c r="BA9" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="AS9" t="s">
+      <c r="BB9" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="AT9" s="3" t="s">
+      <c r="BC9" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="AU9" t="s">
+      <c r="BD9" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="AV9" t="s">
+      <c r="BE9" t="s">
         <v>455</v>
       </c>
-      <c r="AW9" t="s">
-        <v>690</v>
-      </c>
-      <c r="AX9" t="s">
-        <v>159</v>
-      </c>
-      <c r="AY9" t="s">
+      <c r="BF9" t="s">
         <v>456</v>
       </c>
-      <c r="AZ9" s="3" t="s">
+      <c r="BG9" t="s">
         <v>457</v>
       </c>
-      <c r="BA9" s="3" t="s">
+      <c r="BH9" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="BB9" s="3" t="s">
+      <c r="BI9" t="s">
         <v>459</v>
       </c>
-      <c r="BC9" s="3" t="s">
+      <c r="BJ9" t="s">
         <v>460</v>
       </c>
-      <c r="BD9" s="3" t="s">
+      <c r="BK9" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="BE9" t="s">
+      <c r="BL9" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="BF9" t="s">
+      <c r="BM9" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="BG9" t="s">
-        <v>464</v>
-      </c>
-      <c r="BH9" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="BI9" t="s">
-        <v>466</v>
-      </c>
-      <c r="BJ9" t="s">
-        <v>467</v>
-      </c>
-      <c r="BK9" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="BL9" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="BM9" s="3" t="s">
-        <v>470</v>
-      </c>
       <c r="BN9" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
     </row>
     <row r="10" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -4431,199 +4431,199 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>464</v>
+      </c>
+      <c r="C10" t="s">
+        <v>465</v>
+      </c>
+      <c r="D10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E10" t="s">
+        <v>713</v>
+      </c>
+      <c r="F10" t="s">
+        <v>466</v>
+      </c>
+      <c r="G10" t="s">
+        <v>588</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="N10" t="s">
+        <v>468</v>
+      </c>
+      <c r="O10" t="s">
+        <v>469</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="Q10" t="s">
         <v>471</v>
       </c>
-      <c r="C10" t="s">
+      <c r="R10" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="S10" t="s">
         <v>472</v>
       </c>
-      <c r="D10" t="s">
-        <v>594</v>
-      </c>
-      <c r="E10" t="s">
-        <v>596</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="T10" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="G10" t="s">
-        <v>601</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>604</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>616</v>
-      </c>
-      <c r="L10" s="3" t="s">
+      <c r="U10" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="V10" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>621</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="W10" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="O10" t="s">
+      <c r="X10" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="Y10" t="s">
         <v>477</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Z10" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA10" t="s">
         <v>478</v>
       </c>
-      <c r="R10" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="S10" t="s">
+      <c r="AB10" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="AC10" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="T10" s="3" t="s">
+      <c r="AD10" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="U10" s="3" t="s">
-        <v>636</v>
-      </c>
-      <c r="V10" s="3" t="s">
+      <c r="AE10" t="s">
         <v>481</v>
       </c>
-      <c r="W10" s="3" t="s">
+      <c r="AF10" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="X10" s="3" t="s">
+      <c r="AG10" t="s">
+        <v>639</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI10" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="AJ10" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="Z10" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA10" t="s">
+      <c r="AK10" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="AB10" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="AC10" s="3" t="s">
+      <c r="AL10" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="AD10" s="3" t="s">
+      <c r="AM10" t="s">
         <v>487</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AN10" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP10" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="AF10" s="3" t="s">
+      <c r="AQ10" t="s">
+        <v>103</v>
+      </c>
+      <c r="AR10" t="s">
         <v>489</v>
       </c>
-      <c r="AG10" t="s">
-        <v>652</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI10" s="3" t="s">
+      <c r="AS10" t="s">
         <v>490</v>
       </c>
-      <c r="AJ10" s="3" t="s">
+      <c r="AT10" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU10" t="s">
         <v>491</v>
       </c>
-      <c r="AK10" s="3" t="s">
+      <c r="AV10" t="s">
         <v>492</v>
       </c>
-      <c r="AL10" s="3" t="s">
+      <c r="AW10" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="AX10" t="s">
         <v>493</v>
       </c>
-      <c r="AM10" t="s">
+      <c r="AY10" t="s">
         <v>494</v>
       </c>
-      <c r="AN10" t="s">
-        <v>101</v>
-      </c>
-      <c r="AO10" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AP10" s="3" t="s">
+      <c r="AZ10" s="3" t="s">
         <v>495</v>
       </c>
-      <c r="AQ10" t="s">
-        <v>104</v>
-      </c>
-      <c r="AR10" t="s">
+      <c r="BA10" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="AS10" t="s">
+      <c r="BB10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="BC10" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="AT10" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AU10" t="s">
+      <c r="BD10" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="AV10" t="s">
+      <c r="BE10" t="s">
+        <v>659</v>
+      </c>
+      <c r="BF10" t="s">
+        <v>115</v>
+      </c>
+      <c r="BG10" t="s">
         <v>499</v>
       </c>
-      <c r="AW10" s="3" t="s">
-        <v>689</v>
-      </c>
-      <c r="AX10" t="s">
+      <c r="BH10" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="AY10" t="s">
+      <c r="BI10" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="BJ10" t="s">
         <v>501</v>
       </c>
-      <c r="AZ10" s="3" t="s">
+      <c r="BK10" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="BA10" s="3" t="s">
+      <c r="BL10" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="BB10" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="BC10" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="BD10" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="BE10" t="s">
-        <v>672</v>
-      </c>
-      <c r="BF10" t="s">
-        <v>116</v>
-      </c>
-      <c r="BG10" t="s">
-        <v>506</v>
-      </c>
-      <c r="BH10" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="BI10" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="BJ10" t="s">
-        <v>508</v>
-      </c>
-      <c r="BK10" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="BL10" s="3" t="s">
-        <v>510</v>
-      </c>
       <c r="BM10" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="BN10" t="s">
-        <v>703</v>
+        <v>690</v>
       </c>
     </row>
     <row r="11" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -4631,199 +4631,199 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="C11" t="s">
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="D11" t="s">
         <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>597</v>
+        <v>714</v>
       </c>
       <c r="F11" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
       <c r="G11" t="s">
+        <v>505</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="N11" t="s">
+        <v>510</v>
+      </c>
+      <c r="O11" t="s">
+        <v>511</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="Q11" t="s">
         <v>512</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="R11" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="S11" t="s">
+        <v>618</v>
+      </c>
+      <c r="T11" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>614</v>
-      </c>
-      <c r="K11" s="3" t="s">
+      <c r="U11" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>193</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF11" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>199</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI11" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AJ11" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK11" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="AL11" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>206</v>
+      </c>
+      <c r="AO11" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AP11" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>208</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>209</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>210</v>
+      </c>
+      <c r="AT11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>211</v>
+      </c>
+      <c r="AV11" t="s">
         <v>515</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="AW11" t="s">
+        <v>675</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>108</v>
+      </c>
+      <c r="AZ11" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>622</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="BA11" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="O11" t="s">
+      <c r="BB11" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="P11" s="3" t="s">
-        <v>625</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="BC11" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="R11" s="3" t="s">
+      <c r="BD11" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="S11" t="s">
-        <v>631</v>
-      </c>
-      <c r="T11" s="3" t="s">
+      <c r="BE11" t="s">
         <v>521</v>
       </c>
-      <c r="U11" s="3" t="s">
-        <v>637</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="X11" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>196</v>
-      </c>
-      <c r="AB11" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="AC11" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="AD11" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>200</v>
-      </c>
-      <c r="AF11" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>202</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>203</v>
-      </c>
-      <c r="AI11" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="AJ11" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="AK11" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="AL11" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>208</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>209</v>
-      </c>
-      <c r="AO11" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="AP11" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AQ11" t="s">
-        <v>211</v>
-      </c>
-      <c r="AR11" t="s">
-        <v>212</v>
-      </c>
-      <c r="AS11" t="s">
-        <v>213</v>
-      </c>
-      <c r="AT11" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>214</v>
-      </c>
-      <c r="AV11" t="s">
+      <c r="BF11" t="s">
         <v>522</v>
       </c>
-      <c r="AW11" t="s">
-        <v>688</v>
-      </c>
-      <c r="AX11" t="s">
-        <v>159</v>
-      </c>
-      <c r="AY11" t="s">
-        <v>109</v>
-      </c>
-      <c r="AZ11" s="3" t="s">
+      <c r="BG11" t="s">
         <v>523</v>
       </c>
-      <c r="BA11" s="3" t="s">
+      <c r="BH11" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="BB11" s="3" t="s">
+      <c r="BI11" t="s">
         <v>525</v>
       </c>
-      <c r="BC11" s="3" t="s">
+      <c r="BJ11" t="s">
         <v>526</v>
       </c>
-      <c r="BD11" s="3" t="s">
+      <c r="BK11" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="BE11" t="s">
+      <c r="BL11" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="BF11" t="s">
+      <c r="BM11" s="3" t="s">
         <v>529</v>
       </c>
-      <c r="BG11" t="s">
-        <v>530</v>
-      </c>
-      <c r="BH11" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="BI11" t="s">
-        <v>532</v>
-      </c>
-      <c r="BJ11" t="s">
-        <v>533</v>
-      </c>
-      <c r="BK11" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="BL11" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="BM11" s="3" t="s">
-        <v>536</v>
-      </c>
       <c r="BN11" t="s">
-        <v>704</v>
+        <v>691</v>
       </c>
     </row>
     <row r="12" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -4831,199 +4831,199 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>530</v>
+      </c>
+      <c r="C12" t="s">
+        <v>581</v>
+      </c>
+      <c r="D12" t="s">
+        <v>373</v>
+      </c>
+      <c r="E12" t="s">
+        <v>715</v>
+      </c>
+      <c r="F12" t="s">
+        <v>531</v>
+      </c>
+      <c r="G12" t="s">
+        <v>589</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="N12" t="s">
         <v>537</v>
       </c>
-      <c r="C12" t="s">
-        <v>591</v>
-      </c>
-      <c r="D12" t="s">
-        <v>379</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="O12" t="s">
         <v>538</v>
       </c>
-      <c r="F12" t="s">
+      <c r="P12" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q12" t="s">
         <v>539</v>
       </c>
-      <c r="G12" t="s">
-        <v>602</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="R12" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="S12" t="s">
         <v>541</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="T12" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="U12" s="3" t="s">
         <v>543</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>623</v>
-      </c>
-      <c r="N12" t="s">
-        <v>545</v>
-      </c>
-      <c r="O12" t="s">
-        <v>546</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>547</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="S12" t="s">
-        <v>549</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>551</v>
-      </c>
       <c r="V12" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="AA12" t="s">
         <v>242</v>
       </c>
-      <c r="W12" s="3" t="s">
+      <c r="AB12" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="X12" s="3" t="s">
+      <c r="AC12" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="AD12" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="Z12" s="3" t="s">
-        <v>646</v>
-      </c>
-      <c r="AA12" t="s">
+      <c r="AE12" t="s">
         <v>246</v>
       </c>
-      <c r="AB12" s="3" t="s">
+      <c r="AF12" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="AC12" s="3" t="s">
+      <c r="AG12" t="s">
         <v>248</v>
       </c>
-      <c r="AD12" s="3" t="s">
+      <c r="AH12" t="s">
         <v>249</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AI12" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="AF12" s="3" t="s">
+      <c r="AJ12" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AK12" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AL12" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="AI12" s="3" t="s">
+      <c r="AM12" t="s">
         <v>254</v>
       </c>
-      <c r="AJ12" s="3" t="s">
+      <c r="AN12" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO12" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="AK12" s="3" t="s">
+      <c r="AP12" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="AL12" s="3" t="s">
+      <c r="AQ12" t="s">
         <v>257</v>
       </c>
-      <c r="AM12" t="s">
+      <c r="AR12" t="s">
         <v>258</v>
       </c>
-      <c r="AN12" t="s">
-        <v>101</v>
-      </c>
-      <c r="AO12" s="3" t="s">
+      <c r="AS12" t="s">
+        <v>105</v>
+      </c>
+      <c r="AT12" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="AP12" s="3" t="s">
+      <c r="AU12" t="s">
         <v>260</v>
       </c>
-      <c r="AQ12" t="s">
+      <c r="AV12" t="s">
         <v>261</v>
       </c>
-      <c r="AR12" t="s">
+      <c r="AW12" t="s">
+        <v>674</v>
+      </c>
+      <c r="AX12" t="s">
         <v>262</v>
       </c>
-      <c r="AS12" t="s">
-        <v>106</v>
-      </c>
-      <c r="AT12" s="3" t="s">
+      <c r="AY12" t="s">
         <v>263</v>
       </c>
-      <c r="AU12" t="s">
+      <c r="AZ12" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="AV12" t="s">
+      <c r="BA12" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="AW12" t="s">
-        <v>687</v>
-      </c>
-      <c r="AX12" t="s">
+      <c r="BB12" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="AY12" t="s">
+      <c r="BC12" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="AZ12" s="3" t="s">
+      <c r="BD12" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="BA12" s="3" t="s">
+      <c r="BE12" t="s">
+        <v>660</v>
+      </c>
+      <c r="BF12" t="s">
         <v>269</v>
       </c>
-      <c r="BB12" s="3" t="s">
+      <c r="BG12" t="s">
         <v>270</v>
       </c>
-      <c r="BC12" s="3" t="s">
+      <c r="BH12" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="BD12" s="3" t="s">
+      <c r="BI12" t="s">
         <v>272</v>
       </c>
-      <c r="BE12" t="s">
-        <v>673</v>
-      </c>
-      <c r="BF12" t="s">
+      <c r="BJ12" t="s">
         <v>273</v>
       </c>
-      <c r="BG12" t="s">
+      <c r="BK12" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="BH12" s="3" t="s">
+      <c r="BL12" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="BI12" t="s">
+      <c r="BM12" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="BJ12" t="s">
-        <v>277</v>
-      </c>
-      <c r="BK12" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="BL12" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="BM12" s="3" t="s">
-        <v>280</v>
-      </c>
       <c r="BN12" t="s">
-        <v>705</v>
+        <v>692</v>
       </c>
     </row>
     <row r="13" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -5031,199 +5031,199 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C13" t="s">
+        <v>582</v>
+      </c>
+      <c r="D13" t="s">
+        <v>544</v>
+      </c>
+      <c r="E13" t="s">
+        <v>716</v>
+      </c>
+      <c r="F13" t="s">
+        <v>545</v>
+      </c>
+      <c r="G13" t="s">
+        <v>590</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="D13" t="s">
+      <c r="I13" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="N13" t="s">
+        <v>551</v>
+      </c>
+      <c r="O13" t="s">
         <v>552</v>
       </c>
-      <c r="E13" t="s">
+      <c r="P13" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="F13" t="s">
+      <c r="Q13" t="s">
         <v>554</v>
       </c>
-      <c r="G13" t="s">
-        <v>603</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>605</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="R13" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="S13" t="s">
         <v>556</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="T13" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="U13" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="N13" t="s">
-        <v>560</v>
-      </c>
-      <c r="O13" t="s">
-        <v>561</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>562</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>563</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>564</v>
-      </c>
-      <c r="S13" t="s">
-        <v>565</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>567</v>
-      </c>
       <c r="V13" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="AC13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD13" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="W13" s="3" t="s">
+      <c r="AE13" t="s">
         <v>295</v>
       </c>
-      <c r="X13" s="3" t="s">
+      <c r="AF13" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="Y13" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z13" s="3" t="s">
-        <v>646</v>
-      </c>
-      <c r="AA13" t="s">
+      <c r="AG13" t="s">
         <v>297</v>
       </c>
-      <c r="AB13" s="3" t="s">
+      <c r="AH13" t="s">
         <v>298</v>
       </c>
-      <c r="AC13" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD13" s="3" t="s">
+      <c r="AI13" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AJ13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL13" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="AF13" s="3" t="s">
+      <c r="AM13" t="s">
+        <v>644</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO13" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="AG13" t="s">
-        <v>302</v>
-      </c>
-      <c r="AH13" t="s">
+      <c r="AP13" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="AQ13" t="s">
         <v>303</v>
       </c>
-      <c r="AI13" s="3" t="s">
+      <c r="AR13" t="s">
         <v>304</v>
       </c>
-      <c r="AJ13" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="AK13" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AL13" s="3" t="s">
+      <c r="AS13" t="s">
         <v>305</v>
       </c>
-      <c r="AM13" t="s">
-        <v>657</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>101</v>
-      </c>
-      <c r="AO13" s="3" t="s">
+      <c r="AT13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU13" t="s">
         <v>306</v>
       </c>
-      <c r="AP13" s="3" t="s">
+      <c r="AV13" t="s">
+        <v>650</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>673</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>307</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>308</v>
+      </c>
+      <c r="AZ13" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="BA13" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="BB13" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="BC13" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="BD13" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="BE13" t="s">
         <v>658</v>
       </c>
-      <c r="AQ13" t="s">
-        <v>308</v>
-      </c>
-      <c r="AR13" t="s">
-        <v>309</v>
-      </c>
-      <c r="AS13" t="s">
-        <v>310</v>
-      </c>
-      <c r="AT13" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>311</v>
-      </c>
-      <c r="AV13" t="s">
-        <v>663</v>
-      </c>
-      <c r="AW13" t="s">
-        <v>686</v>
-      </c>
-      <c r="AX13" t="s">
-        <v>312</v>
-      </c>
-      <c r="AY13" t="s">
+      <c r="BF13" t="s">
         <v>313</v>
       </c>
-      <c r="AZ13" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="BA13" s="3" t="s">
+      <c r="BG13" t="s">
+        <v>577</v>
+      </c>
+      <c r="BH13" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="BB13" s="3" t="s">
+      <c r="BI13" t="s">
         <v>316</v>
       </c>
-      <c r="BC13" s="3" t="s">
+      <c r="BJ13" t="s">
         <v>317</v>
       </c>
-      <c r="BD13" s="3" t="s">
-        <v>669</v>
-      </c>
-      <c r="BE13" t="s">
-        <v>671</v>
-      </c>
-      <c r="BF13" t="s">
+      <c r="BK13" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="BG13" t="s">
-        <v>587</v>
-      </c>
-      <c r="BH13" s="3" t="s">
+      <c r="BL13" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="BM13" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="BI13" t="s">
-        <v>321</v>
-      </c>
-      <c r="BJ13" t="s">
-        <v>322</v>
-      </c>
-      <c r="BK13" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="BL13" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="BM13" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="BN13" t="s">
-        <v>706</v>
+        <v>693</v>
       </c>
     </row>
     <row r="14" spans="1:66" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -5231,254 +5231,254 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>559</v>
+      </c>
+      <c r="C14" t="s">
+        <v>583</v>
+      </c>
+      <c r="D14" t="s">
+        <v>560</v>
+      </c>
+      <c r="E14" t="s">
+        <v>717</v>
+      </c>
+      <c r="F14" t="s">
+        <v>561</v>
+      </c>
+      <c r="G14" t="s">
+        <v>562</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="N14" t="s">
         <v>568</v>
       </c>
-      <c r="C14" t="s">
-        <v>593</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="O14" t="s">
         <v>569</v>
       </c>
-      <c r="E14" t="s">
+      <c r="P14" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="F14" t="s">
+      <c r="Q14" t="s">
         <v>571</v>
       </c>
-      <c r="G14" t="s">
+      <c r="R14" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>606</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="S14" t="s">
         <v>573</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="T14" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="U14" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>575</v>
-      </c>
-      <c r="L14" s="3" t="s">
+      <c r="V14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z14" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="AC14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF14" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>343</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>344</v>
+      </c>
+      <c r="AI14" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="AJ14" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="AK14" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="AL14" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>348</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>349</v>
+      </c>
+      <c r="AO14" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="AP14" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>352</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>353</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>354</v>
+      </c>
+      <c r="AT14" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>357</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>672</v>
+      </c>
+      <c r="AX14" t="s">
         <v>576</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="AY14" t="s">
+        <v>358</v>
+      </c>
+      <c r="AZ14" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="BA14" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="BB14" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="BC14" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="BD14" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="BE14" t="s">
+        <v>363</v>
+      </c>
+      <c r="BF14" t="s">
+        <v>364</v>
+      </c>
+      <c r="BG14" t="s">
+        <v>365</v>
+      </c>
+      <c r="BH14" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="BI14" t="s">
+        <v>367</v>
+      </c>
+      <c r="BJ14" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK14" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="BL14" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="BM14" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="O14" t="s">
-        <v>579</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>580</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>581</v>
-      </c>
-      <c r="R14" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="S14" t="s">
-        <v>583</v>
-      </c>
-      <c r="T14" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="U14" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="V14" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="W14" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="X14" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z14" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB14" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="AC14" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD14" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF14" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>349</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>350</v>
-      </c>
-      <c r="AI14" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="AJ14" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="AK14" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="AL14" s="3" t="s">
-        <v>655</v>
-      </c>
-      <c r="AM14" t="s">
-        <v>354</v>
-      </c>
-      <c r="AN14" t="s">
-        <v>355</v>
-      </c>
-      <c r="AO14" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="AP14" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="AQ14" t="s">
-        <v>358</v>
-      </c>
-      <c r="AR14" t="s">
-        <v>359</v>
-      </c>
-      <c r="AS14" t="s">
-        <v>360</v>
-      </c>
-      <c r="AT14" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>362</v>
-      </c>
-      <c r="AV14" t="s">
-        <v>363</v>
-      </c>
-      <c r="AW14" t="s">
-        <v>685</v>
-      </c>
-      <c r="AX14" t="s">
-        <v>586</v>
-      </c>
-      <c r="AY14" t="s">
-        <v>364</v>
-      </c>
-      <c r="AZ14" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="BA14" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="BB14" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="BC14" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="BD14" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="BE14" t="s">
-        <v>369</v>
-      </c>
-      <c r="BF14" t="s">
-        <v>370</v>
-      </c>
-      <c r="BG14" t="s">
-        <v>371</v>
-      </c>
-      <c r="BH14" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="BI14" t="s">
-        <v>373</v>
-      </c>
-      <c r="BJ14" t="s">
-        <v>374</v>
-      </c>
-      <c r="BK14" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="BL14" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="BM14" s="3" t="s">
-        <v>588</v>
-      </c>
       <c r="BN14" t="s">
-        <v>707</v>
+        <v>694</v>
       </c>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.2">
       <c r="BN15" t="s">
-        <v>708</v>
+        <v>695</v>
       </c>
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.2">
       <c r="BN16" t="s">
-        <v>709</v>
+        <v>696</v>
       </c>
     </row>
     <row r="17" spans="66:66" x14ac:dyDescent="0.2">
       <c r="BN17" t="s">
-        <v>710</v>
+        <v>697</v>
       </c>
     </row>
     <row r="18" spans="66:66" x14ac:dyDescent="0.2">
       <c r="BN18" t="s">
-        <v>711</v>
+        <v>698</v>
       </c>
     </row>
     <row r="19" spans="66:66" x14ac:dyDescent="0.2">
       <c r="BN19" t="s">
-        <v>712</v>
+        <v>699</v>
       </c>
     </row>
     <row r="20" spans="66:66" x14ac:dyDescent="0.2">
       <c r="BN20" t="s">
-        <v>713</v>
+        <v>700</v>
       </c>
     </row>
     <row r="21" spans="66:66" x14ac:dyDescent="0.2">
       <c r="BN21" t="s">
-        <v>714</v>
+        <v>701</v>
       </c>
     </row>
     <row r="22" spans="66:66" x14ac:dyDescent="0.2">
       <c r="BN22" t="s">
-        <v>715</v>
+        <v>702</v>
       </c>
     </row>
     <row r="23" spans="66:66" x14ac:dyDescent="0.2">
       <c r="BN23" t="s">
-        <v>716</v>
+        <v>703</v>
       </c>
     </row>
     <row r="24" spans="66:66" x14ac:dyDescent="0.2">
       <c r="BN24" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
     </row>
     <row r="25" spans="66:66" x14ac:dyDescent="0.2">
       <c r="BN25" t="s">
-        <v>718</v>
+        <v>705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>